<commit_message>
Finish off applying descriptive stats
</commit_message>
<xml_diff>
--- a/Applying Descriptive Statistics/Demonstration Descriptive statistics formulas.xlsx
+++ b/Applying Descriptive Statistics/Demonstration Descriptive statistics formulas.xlsx
@@ -1,43 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Friedturnip\Desktop\Data Foundations BUILD\Applying Basic Statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\Data_Foundations_WithYouWithMe\Applying Descriptive Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{968A95F3-3F83-4A1B-A826-B387632BFF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76C4198-6B90-4619-9C20-EA6974AFE7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="630" windowWidth="27675" windowHeight="14145" activeTab="1" xr2:uid="{8DC780A2-5CD9-4C57-9681-988DB506AD76}"/>
+    <workbookView xWindow="3780" yWindow="630" windowWidth="24690" windowHeight="14805" activeTab="1" xr2:uid="{8DC780A2-5CD9-4C57-9681-988DB506AD76}"/>
   </bookViews>
   <sheets>
     <sheet name="Excel Formulas" sheetId="2" r:id="rId1"/>
     <sheet name="Descriptive Statistics" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Descriptive Statistics'!$A$2:$D$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Descriptive Statistics'!$A$1:$A$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Salary</t>
   </si>
@@ -109,14 +101,18 @@
   </si>
   <si>
     <t>Excel Formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $65,308.18 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -223,40 +219,40 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -572,7 +568,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6453D79B-905B-49C2-B992-C6BCE32F56B2}">
-  <dimension ref="B2:K16"/>
+  <dimension ref="B2:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16:E16"/>
@@ -584,34 +580,29 @@
     <col min="6" max="6" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="13" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="10"/>
+      <c r="D5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -624,61 +615,60 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="16" t="s">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="16" t="s">
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="12"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>22</v>
       </c>
@@ -691,10 +681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42CE3DC1-CB93-4809-A03D-EF721E8AA11B}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,108 +695,137 @@
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>62156</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="15"/>
+      <c r="F2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>64215</v>
+        <v>63152</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="5">
+        <f>AVERAGE(A2:A12)</f>
+        <v>65308.181818181816</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>66604</v>
+        <v>63152</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <f>_xlfn.MODE.SNGL(A2:A12)</f>
+        <v>66604</v>
+      </c>
+      <c r="F4" s="2">
+        <f>_xlfn.MODE.SNGL(A2:A12)</f>
+        <v>66604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>66987</v>
+        <v>64215</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="16">
+        <f>MEDIAN(A2:A12)</f>
+        <v>66156</v>
+      </c>
+      <c r="F5" s="4">
+        <f>MEDIAN(A2:A12)</f>
+        <v>66156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>66604</v>
+        <v>66156</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="17">
+        <f>A12-A2</f>
+        <v>4831</v>
+      </c>
+      <c r="F6" s="18">
+        <f>A12-A2</f>
+        <v>4831</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>66604</v>
+        <v>66156</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>66604</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>63152</v>
+        <v>66604</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>63152</v>
+        <v>66604</v>
       </c>
       <c r="B10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>66156</v>
+        <v>66604</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>66156</v>
+        <v>66987</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A12" xr:uid="{42CE3DC1-CB93-4809-A03D-EF721E8AA11B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A12">
+      <sortCondition ref="A1:A12"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="C2:D2"/>
   </mergeCells>

</xml_diff>